<commit_message>
cleanup from the sprint6 merge
</commit_message>
<xml_diff>
--- a/public/CSV Import.xlsx
+++ b/public/CSV Import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14120" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata fields for import" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>73-019-1--73-019-8</t>
-  </si>
-  <si>
-    <t>CSHM</t>
   </si>
   <si>
     <t>Ampex 631</t>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>ORAL HISTORY INTERVIEWS OF</t>
+  </si>
+  <si>
+    <t>B-CSHM</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -436,6 +436,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -474,6 +476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -486,9 +489,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="38">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -506,6 +508,7 @@
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -523,6 +526,7 @@
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="9"/>
   </cellStyles>
@@ -855,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H4" sqref="H3:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -868,7 +872,7 @@
     <col min="5" max="5" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -900,92 +904,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="23" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="5" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
     </row>
     <row r="2" spans="1:35" ht="24" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>7</v>
@@ -994,61 +998,61 @@
         <v>8</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="AB2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="AD2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="60">
@@ -1068,82 +1072,82 @@
         <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J3" s="1">
         <v>1973</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="N3" s="1">
         <v>5297141</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="Q3" s="1">
         <v>50488261</v>
       </c>
       <c r="S3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB3" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="AC3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AH3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI3" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="45">
@@ -1154,37 +1158,37 @@
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="J4" s="1">
         <v>1969</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="N4" s="1">
         <v>4938795</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="Q4" s="1">
         <v>47794774</v>
@@ -1193,10 +1197,10 @@
         <v>1</v>
       </c>
       <c r="U4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1236,52 +1240,52 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="90">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="105">
       <c r="A3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45">
       <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1300,7 +1304,7 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1314,28 +1318,28 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -1344,13 +1348,13 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>47</v>
-      </c>
-      <c r="N1" t="s">
-        <v>48</v>
       </c>
       <c r="O1" t="s">
         <v>7</v>
@@ -1359,32 +1363,32 @@
         <v>8</v>
       </c>
       <c r="Q1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="8">
+        <v>76</v>
+      </c>
+      <c r="B2" s="4">
         <v>40000000000002</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="4">
         <v>30000000000004</v>
       </c>
       <c r="D2" t="s">
@@ -1399,94 +1403,94 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
+      <c r="H2" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J2">
         <v>1973</v>
       </c>
       <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
         <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
       </c>
       <c r="N2">
         <v>5297141</v>
       </c>
       <c r="O2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
         <v>17</v>
-      </c>
-      <c r="P2" t="s">
-        <v>18</v>
       </c>
       <c r="Q2">
         <v>50488261</v>
       </c>
       <c r="S2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="8">
+        <v>76</v>
+      </c>
+      <c r="B3" s="4">
         <v>40000000000010</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="4">
         <v>30000000000012</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
+      <c r="H3" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J3">
         <v>1969</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
         <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
       </c>
       <c r="N3">
         <v>4938795</v>
       </c>
       <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
         <v>33</v>
-      </c>
-      <c r="P3" t="s">
-        <v>34</v>
       </c>
       <c r="Q3">
         <v>47794774</v>
@@ -1495,13 +1499,13 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
+        <v>80</v>
+      </c>
+      <c r="T3" t="s">
         <v>81</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>82</v>
-      </c>
-      <c r="V3" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1519,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1539,43 +1543,43 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>47</v>
-      </c>
-      <c r="N1" t="s">
-        <v>48</v>
       </c>
       <c r="O1" t="s">
         <v>7</v>
@@ -1584,29 +1588,29 @@
         <v>8</v>
       </c>
       <c r="Q1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="30">
       <c r="A2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="8">
+        <v>88</v>
+      </c>
+      <c r="B2" s="4">
         <v>40000000000002</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="4">
         <v>30000000000004</v>
       </c>
       <c r="D2" t="s">
@@ -1621,91 +1625,91 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
+      <c r="H2" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J2">
         <v>1973</v>
       </c>
       <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
         <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
       </c>
       <c r="N2">
         <v>5297141</v>
       </c>
       <c r="O2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
         <v>17</v>
-      </c>
-      <c r="P2" t="s">
-        <v>18</v>
       </c>
       <c r="Q2">
         <v>50488261</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="8">
+        <v>88</v>
+      </c>
+      <c r="B3" s="4">
         <v>40000000000010</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="4">
         <v>30000000000012</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
+      <c r="H3" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J3">
         <v>1969</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
         <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
       </c>
       <c r="N3">
         <v>4938795</v>
       </c>
       <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
         <v>33</v>
-      </c>
-      <c r="P3" t="s">
-        <v>34</v>
       </c>
       <c r="Q3">
         <v>47794774</v>
@@ -1714,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1732,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1744,7 +1748,7 @@
     <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -1768,43 +1772,43 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>7</v>
@@ -1813,47 +1817,47 @@
         <v>8</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="28" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="4">
         <v>40000000000002</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="4">
         <v>30000000000004</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1869,108 +1873,108 @@
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J2" s="1">
         <v>1973</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="N2" s="1">
         <v>5297141</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q2" s="1">
         <v>50488261</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="30">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="4">
         <v>40000000000010</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="4">
         <v>30000000000012</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1">
         <v>1969</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="N3" s="1">
         <v>4938795</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q3" s="1">
         <v>47794774</v>
@@ -1981,10 +1985,10 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>

</xml_diff>